<commit_message>
Added instagram_scraping function using instaloader library to call instagram api to get posts from profile
</commit_message>
<xml_diff>
--- a/url.xlsx
+++ b/url.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IA_AWEEYIAL\Documents\Intern\SocialCrawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E95F8B-EBFB-4E3D-AE48-4A675EA3D509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B1951A-56DE-402F-99B3-A90A155E089B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{4F07DC25-6319-43F9-B3AA-A1450DAD6F96}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>url</t>
   </si>
   <si>
     <t>https://www.dsta.gov.sg/home</t>
+  </si>
+  <si>
+    <t>https://www.tech.gov.sg/</t>
   </si>
 </sst>
 </file>
@@ -86,11 +89,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FF2C04-FED6-4DFC-A345-69BAAB0A0211}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,22 +431,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{2718574F-094D-4A51-9963-D3964B1645CE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FA0552D3C74FC4BB89A19565DD4C5FC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6fb3863651fa8bfa98bd1564a381b1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0bcc9261-9a97-47e5-beba-c48027403af5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23afa1852b5595dfe4f0ad81ee998a28" ns3:_="">
     <xsd:import namespace="0bcc9261-9a97-47e5-beba-c48027403af5"/>
@@ -588,6 +591,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -595,14 +607,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F23F213A-46E3-4D57-9AC3-3A57BB260FA0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11B0ED41-072C-49AE-AE61-284CF3FA7E52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -620,6 +624,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F23F213A-46E3-4D57-9AC3-3A57BB260FA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E09972C1-E9BA-41D5-B384-D163DEBBB073}">
   <ds:schemaRefs>

</xml_diff>